<commit_message>
Level 9 with translations
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="translation_template" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="translations" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="209">
   <si>
     <t>Key</t>
   </si>
@@ -290,30 +290,6 @@
   </si>
   <si>
     <t>Нажмите Новую Кнопку</t>
-  </si>
-  <si>
-    <t>GANDU</t>
-  </si>
-  <si>
-    <t>X Marks the Spot o' Trouble</t>
-  </si>
-  <si>
-    <t>Launch the Chaos 🚀🎲</t>
-  </si>
-  <si>
-    <t>Start_Game</t>
-  </si>
-  <si>
-    <t>Weigh Anchor!</t>
-  </si>
-  <si>
-    <t>Let It All Fade to Black 🎭🕳</t>
-  </si>
-  <si>
-    <t>End_Game</t>
-  </si>
-  <si>
-    <t>Return to Port</t>
   </si>
   <si>
     <t>FIRST_LEVEL_TIP</t>
@@ -412,6 +388,9 @@
     <t>START_GAME</t>
   </si>
   <si>
+    <t>Hoist the Sails!</t>
+  </si>
+  <si>
     <t>Start Game</t>
   </si>
   <si>
@@ -421,6 +400,9 @@
     <t>BACK_TO_START</t>
   </si>
   <si>
+    <t>Return to Port</t>
+  </si>
+  <si>
     <t>Back to Start</t>
   </si>
   <si>
@@ -430,6 +412,9 @@
     <t>END_GAME</t>
   </si>
   <si>
+    <t>Walk the Plank!</t>
+  </si>
+  <si>
     <t>End Game</t>
   </si>
   <si>
@@ -439,6 +424,9 @@
     <t>CONTINUE</t>
   </si>
   <si>
+    <t>The Journey Ain’t Over!</t>
+  </si>
+  <si>
     <t>Continue</t>
   </si>
   <si>
@@ -586,7 +574,7 @@
     <t>Introduction</t>
   </si>
   <si>
-    <t>Вступлеие</t>
+    <t>Вступление</t>
   </si>
   <si>
     <t>jumpL2</t>
@@ -644,6 +632,15 @@
   </si>
   <si>
     <t>Двойная проблема</t>
+  </si>
+  <si>
+    <t>dontblockmeL9</t>
+  </si>
+  <si>
+    <t>Don't block me!</t>
+  </si>
+  <si>
+    <t>Пропустите!</t>
   </si>
 </sst>
 </file>
@@ -899,9 +896,6 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="19.25"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -1224,137 +1218,135 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="1" t="s">
+    <row r="32">
+      <c r="A32" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="1" t="s">
+    <row r="33">
+      <c r="A33" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="1" t="s">
+    <row r="34">
+      <c r="A34" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>100</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="1" t="s">
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C37" s="1" t="s">
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C38" s="1" t="s">
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>112</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>128</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -1364,336 +1356,326 @@
         <v>130</v>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C51" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D52" s="1" t="s">
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="s">
         <v>142</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>186</v>
+        <v>115</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>187</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>123</v>
+        <v>195</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>124</v>
+        <v>196</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>206</v>
+        <v>166</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>209</v>
+        <v>169</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>